<commit_message>
Melhora qualificação Maps, UX de seleção e proxy de atividade
</commit_message>
<xml_diff>
--- a/prospeccao_instagram_locator.xlsx
+++ b/prospeccao_instagram_locator.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="prospeccao" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'prospeccao'!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'prospeccao'!$A$1:$S$27</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -437,24 +437,24 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="16" customWidth="1" min="1" max="1"/>
-    <col width="7" customWidth="1" min="2" max="2"/>
-    <col width="6" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="28" customWidth="1" min="3" max="3"/>
+    <col width="55" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
     <col width="6" customWidth="1" min="7" max="7"/>
     <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="6" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
     <col width="8" customWidth="1" min="10" max="10"/>
-    <col width="7" customWidth="1" min="11" max="11"/>
+    <col width="26" customWidth="1" min="11" max="11"/>
     <col width="17" customWidth="1" min="12" max="12"/>
     <col width="10" customWidth="1" min="13" max="13"/>
     <col width="22" customWidth="1" min="14" max="14"/>
     <col width="7" customWidth="1" min="15" max="15"/>
-    <col width="12" customWidth="1" min="16" max="16"/>
-    <col width="13" customWidth="1" min="17" max="17"/>
+    <col width="60" customWidth="1" min="16" max="16"/>
+    <col width="55" customWidth="1" min="17" max="17"/>
     <col width="8" customWidth="1" min="18" max="18"/>
-    <col width="13" customWidth="1" min="19" max="19"/>
+    <col width="27" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -554,8 +554,1854 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>alessandradesign_</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alessandradesign_/</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/alessandradesign_/</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:54:25+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>bbrows_design</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bbrows_design/</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bbrows_design/</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>bfsobrancelhas</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bfsobrancelhas/</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/bfsobrancelhas/</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>elenamorales_beautycenter</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/elenamorales_beautycenter/</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/elenamorales_beautycenter/</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>eyebrowdesignporto</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/eyebrowdesignporto/</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/eyebrowdesignporto/</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fernanda.sobrancelhas</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fernanda.sobrancelhas/</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/fernanda.sobrancelhas/</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>gabrielasobrancelhas</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/gabrielasobrancelhas/</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/gabrielasobrancelhas/</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>giselebiazottopmu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/giselebiazottopmu/</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/giselebiazottopmu/</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>jessicabeautyacademy</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/jessicabeautyacademy/</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/jessicabeautyacademy/</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>lindasouzasobrancelhas</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/lindasouzasobrancelhas/</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/lindasouzasobrancelhas/</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>michellyalvesdesigner</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/michellyalvesdesigner/</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/michellyalvesdesigner/</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nataliabeauty</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nataliabeauty/</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nataliabeauty/</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nathaliabatistadesigner</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nathaliabatistadesigner/</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nathaliabatistadesigner/</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nicoly_portugal</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nicoly_portugal/</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/nicoly_portugal/</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>rs.designer.de.sobrancelha</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/rs.designer.de.sobrancelha/</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/rs.designer.de.sobrancelha/</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sdtijucauruguai</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sdtijucauruguai/</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sdtijucauruguai/</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>sobrancelhadelas</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhadelas/</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhadelas/</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>sobrancelhamarcada</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhamarcada/</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhamarcada/</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>4</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>sobrancelhas.forever</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.forever/</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.forever/</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>4</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>sobrancelhas.portugal</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.portugal/</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.portugal/</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>sobrancelhas.store</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.store/</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhas.store/</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>sobrancelhasderainha</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasderainha/</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasderainha/</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>sobrancelhasdesign</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasdesign/</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasdesign/</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sobrancelhasdesignsantarem</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasdesignsantarem/</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: designer de sobrancelhas Portugal perfil instagram</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/sobrancelhasdesignsantarem/</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>studiojoicevalle</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/studiojoicevalle/</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/studiojoicevalle/</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>4</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Instagram</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>studioleialiberato</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/studioleialiberato/</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>designer de sobrancelhas</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>IG Locator | Bio nao verificada (modo rapido). Encontrado por: site:instagram.com designer de sobrancelhas Portugal instagram</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/studioleialiberato/</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>novo</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>2026-02-12T19:45:24+00:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:S1"/>
+  <autoFilter ref="A1:S27"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>